<commit_message>
Job creation and posting
</commit_message>
<xml_diff>
--- a/public/JobCreationTemplate.xlsx
+++ b/public/JobCreationTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8555"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Job Requisition" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Position Title</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>it</t>
   </si>
   <si>
     <t>Responsible for backend development</t>
@@ -1158,8 +1155,8 @@
   <sheetPr/>
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1243,8 +1240,8 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1259,10 +1256,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1283,22 +1280,22 @@
         <v>3</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
         <v>28</v>
-      </c>
-      <c r="S2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>29</v>
       </c>
       <c r="U2">
         <v>1</v>
@@ -1308,8 +1305,8 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -1324,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1348,22 +1345,22 @@
         <v>3</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>27</v>
       </c>
-      <c r="R3" t="s">
-        <v>28</v>
-      </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U3">
         <v>1</v>

</xml_diff>

<commit_message>
remove validation in JobCreation
</commit_message>
<xml_diff>
--- a/public/JobCreationTemplate.xlsx
+++ b/public/JobCreationTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8555"/>
   </bookViews>
   <sheets>
     <sheet name="Job Requisition" sheetId="1" r:id="rId1"/>
@@ -62,16 +62,16 @@
     <t>Eligibility Age Max</t>
   </si>
   <si>
+    <t>Probation Period</t>
+  </si>
+  <si>
+    <t>Documents Required</t>
+  </si>
+  <si>
     <t>Mandatory Experience</t>
   </si>
   <si>
     <t>Preferred Experience</t>
-  </si>
-  <si>
-    <t>Probation Period</t>
-  </si>
-  <si>
-    <t>Documents Required</t>
   </si>
   <si>
     <t>Min Credit Score</t>
@@ -1155,8 +1155,8 @@
   <sheetPr/>
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1165,7 +1165,9 @@
     <col min="2" max="2" width="19.2222222222222" customWidth="1"/>
     <col min="3" max="8" width="35" customWidth="1"/>
     <col min="10" max="10" width="14.3333333333333" customWidth="1"/>
-    <col min="15" max="15" width="35" customWidth="1"/>
+    <col min="13" max="13" width="35" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
+    <col min="15" max="15" width="28.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="19.4444444444444" customWidth="1"/>
     <col min="18" max="18" width="23.4444444444444" customWidth="1"/>
     <col min="20" max="20" width="17.5555555555556" customWidth="1"/>
@@ -1270,17 +1272,17 @@
       <c r="K2" s="3">
         <v>30</v>
       </c>
-      <c r="L2" s="3">
-        <v>2</v>
-      </c>
-      <c r="M2" s="3">
-        <v>4</v>
-      </c>
-      <c r="N2">
+      <c r="L2">
         <v>3</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="N2" s="2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>1.5</v>
       </c>
       <c r="P2" t="s">
         <v>25</v>
@@ -1335,17 +1337,17 @@
       <c r="K3" s="3">
         <v>30</v>
       </c>
-      <c r="L3" s="3">
-        <v>2</v>
-      </c>
-      <c r="M3" s="3">
-        <v>4</v>
-      </c>
-      <c r="N3">
+      <c r="L3">
         <v>3</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>1.5</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
@@ -1366,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1" spans="3:15">
+    <row r="4" ht="30" customHeight="1" spans="3:14">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1376,11 +1378,10 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" ht="30" customHeight="1" spans="3:15">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="3:14">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1390,11 +1391,10 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" ht="30" customHeight="1" spans="3:15">
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="3:14">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1404,11 +1404,10 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" ht="30" customHeight="1" spans="3:15">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="3:14">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1418,11 +1417,10 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" ht="30" customHeight="1" spans="3:15">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="3:14">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1432,11 +1430,10 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" ht="30" customHeight="1" spans="3:15">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="3:14">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1446,11 +1443,10 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" ht="30" customHeight="1" spans="3:15">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="3:14">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1460,11 +1456,10 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" ht="30" customHeight="1" spans="3:15">
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="3:14">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1474,11 +1469,10 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" ht="30" customHeight="1" spans="3:15">
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="3:14">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1488,11 +1482,10 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" ht="30" customHeight="1" spans="3:15">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="3:14">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1502,11 +1495,10 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" ht="30" customHeight="1" spans="3:15">
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" ht="30" customHeight="1" spans="3:14">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1516,11 +1508,10 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" ht="30" customHeight="1" spans="3:15">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" ht="30" customHeight="1" spans="3:14">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1530,11 +1521,10 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" ht="30" customHeight="1" spans="3:15">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" ht="30" customHeight="1" spans="3:14">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1544,11 +1534,10 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" ht="30" customHeight="1" spans="3:15">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" ht="30" customHeight="1" spans="3:14">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1558,11 +1547,10 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" ht="30" customHeight="1" spans="3:15">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" ht="30" customHeight="1" spans="3:14">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1572,11 +1560,10 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" ht="30" customHeight="1" spans="3:15">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" ht="30" customHeight="1" spans="3:14">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1586,11 +1573,10 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" ht="30" customHeight="1" spans="3:15">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" ht="30" customHeight="1" spans="3:14">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1600,11 +1586,10 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" ht="30" customHeight="1" spans="3:15">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" ht="30" customHeight="1" spans="3:14">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1614,11 +1599,10 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" ht="30" customHeight="1" spans="3:15">
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" ht="30" customHeight="1" spans="3:14">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1628,11 +1612,10 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" ht="30" customHeight="1" spans="3:15">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" ht="30" customHeight="1" spans="3:14">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1642,11 +1625,10 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" ht="30" customHeight="1" spans="3:15">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" ht="30" customHeight="1" spans="3:14">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1656,11 +1638,10 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" ht="30" customHeight="1" spans="3:15">
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" ht="30" customHeight="1" spans="3:14">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1670,11 +1651,10 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" ht="30" customHeight="1" spans="3:15">
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" ht="30" customHeight="1" spans="3:14">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1684,11 +1664,10 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" ht="30" customHeight="1" spans="3:15">
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" ht="30" customHeight="1" spans="3:14">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1698,11 +1677,10 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" ht="30" customHeight="1" spans="3:15">
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" ht="30" customHeight="1" spans="3:14">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1712,11 +1690,10 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" ht="30" customHeight="1" spans="3:15">
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" ht="30" customHeight="1" spans="3:14">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1726,11 +1703,10 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="O29" s="2"/>
-    </row>
-    <row r="30" ht="30" customHeight="1" spans="3:15">
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" ht="30" customHeight="1" spans="3:14">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1740,11 +1716,10 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" ht="30" customHeight="1" spans="3:15">
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" ht="30" customHeight="1" spans="3:14">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1754,11 +1729,10 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="O31" s="2"/>
-    </row>
-    <row r="32" ht="30" customHeight="1" spans="3:15">
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" ht="30" customHeight="1" spans="3:14">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1768,11 +1742,10 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="O32" s="2"/>
-    </row>
-    <row r="33" ht="30" customHeight="1" spans="3:15">
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" ht="30" customHeight="1" spans="3:14">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1782,11 +1755,10 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="O33" s="2"/>
-    </row>
-    <row r="34" ht="30" customHeight="1" spans="3:15">
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" ht="30" customHeight="1" spans="3:14">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1796,11 +1768,10 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="O34" s="2"/>
-    </row>
-    <row r="35" ht="30" customHeight="1" spans="3:15">
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" ht="30" customHeight="1" spans="3:14">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1810,11 +1781,10 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="O35" s="2"/>
-    </row>
-    <row r="36" ht="30" customHeight="1" spans="3:15">
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" ht="30" customHeight="1" spans="3:14">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1824,11 +1794,10 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="O36" s="2"/>
-    </row>
-    <row r="37" ht="30" customHeight="1" spans="3:15">
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" ht="30" customHeight="1" spans="3:14">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1838,11 +1807,10 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="O37" s="2"/>
-    </row>
-    <row r="38" ht="30" customHeight="1" spans="3:15">
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" ht="30" customHeight="1" spans="3:14">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1852,11 +1820,10 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="O38" s="2"/>
-    </row>
-    <row r="39" ht="30" customHeight="1" spans="3:15">
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" ht="30" customHeight="1" spans="3:14">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1866,11 +1833,10 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="O39" s="2"/>
-    </row>
-    <row r="40" ht="30" customHeight="1" spans="3:15">
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" ht="30" customHeight="1" spans="3:14">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1880,11 +1846,10 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="O40" s="2"/>
-    </row>
-    <row r="41" ht="30" customHeight="1" spans="3:15">
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" ht="30" customHeight="1" spans="3:14">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1894,11 +1859,10 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="O41" s="2"/>
-    </row>
-    <row r="42" ht="30" customHeight="1" spans="3:15">
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" ht="30" customHeight="1" spans="3:14">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1908,11 +1872,10 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="O42" s="2"/>
-    </row>
-    <row r="43" ht="30" customHeight="1" spans="3:15">
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" ht="30" customHeight="1" spans="3:14">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1922,11 +1885,10 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="O43" s="2"/>
-    </row>
-    <row r="44" ht="30" customHeight="1" spans="3:15">
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" ht="30" customHeight="1" spans="3:14">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1936,11 +1898,10 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="O44" s="2"/>
-    </row>
-    <row r="45" ht="30" customHeight="1" spans="3:15">
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" ht="30" customHeight="1" spans="3:14">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1950,11 +1911,10 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="O45" s="2"/>
-    </row>
-    <row r="46" ht="30" customHeight="1" spans="3:15">
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" ht="30" customHeight="1" spans="3:14">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1964,11 +1924,10 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="O46" s="2"/>
-    </row>
-    <row r="47" ht="30" customHeight="1" spans="3:15">
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" ht="30" customHeight="1" spans="3:14">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1978,11 +1937,10 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="O47" s="2"/>
-    </row>
-    <row r="48" ht="30" customHeight="1" spans="3:15">
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" ht="30" customHeight="1" spans="3:14">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1992,11 +1950,10 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="O48" s="2"/>
-    </row>
-    <row r="49" ht="30" customHeight="1" spans="3:15">
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" ht="30" customHeight="1" spans="3:14">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2006,11 +1963,10 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="O49" s="2"/>
-    </row>
-    <row r="50" ht="30" customHeight="1" spans="3:15">
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" ht="30" customHeight="1" spans="3:14">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2020,11 +1976,10 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="O50" s="2"/>
-    </row>
-    <row r="51" ht="30" customHeight="1" spans="3:15">
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" ht="30" customHeight="1" spans="3:14">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2034,11 +1989,10 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="O51" s="2"/>
-    </row>
-    <row r="52" ht="30" customHeight="1" spans="3:15">
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" ht="30" customHeight="1" spans="3:14">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2048,11 +2002,10 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="O52" s="2"/>
-    </row>
-    <row r="53" ht="30" customHeight="1" spans="3:15">
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" ht="30" customHeight="1" spans="3:14">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2062,11 +2015,10 @@
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="O53" s="2"/>
-    </row>
-    <row r="54" ht="30" customHeight="1" spans="3:15">
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" ht="30" customHeight="1" spans="3:14">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2076,11 +2028,10 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="O54" s="2"/>
-    </row>
-    <row r="55" ht="30" customHeight="1" spans="3:15">
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" ht="30" customHeight="1" spans="3:14">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2090,11 +2041,10 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="O55" s="2"/>
-    </row>
-    <row r="56" ht="30" customHeight="1" spans="3:15">
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+    </row>
+    <row r="56" ht="30" customHeight="1" spans="3:14">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2104,11 +2054,10 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="O56" s="2"/>
-    </row>
-    <row r="57" ht="30" customHeight="1" spans="3:15">
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+    </row>
+    <row r="57" ht="30" customHeight="1" spans="3:14">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2118,11 +2067,10 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="O57" s="2"/>
-    </row>
-    <row r="58" ht="30" customHeight="1" spans="3:15">
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" ht="30" customHeight="1" spans="3:14">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2132,11 +2080,10 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="O58" s="2"/>
-    </row>
-    <row r="59" ht="30" customHeight="1" spans="3:15">
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" ht="30" customHeight="1" spans="3:14">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -2146,11 +2093,10 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="O59" s="2"/>
-    </row>
-    <row r="60" ht="30" customHeight="1" spans="3:15">
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" ht="30" customHeight="1" spans="3:14">
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -2160,11 +2106,10 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="O60" s="2"/>
-    </row>
-    <row r="61" ht="30" customHeight="1" spans="3:15">
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" ht="30" customHeight="1" spans="3:14">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -2174,11 +2119,10 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="O61" s="2"/>
-    </row>
-    <row r="62" ht="30" customHeight="1" spans="3:15">
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+    </row>
+    <row r="62" ht="30" customHeight="1" spans="3:14">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -2188,11 +2132,10 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="O62" s="2"/>
-    </row>
-    <row r="63" ht="30" customHeight="1" spans="3:15">
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+    </row>
+    <row r="63" ht="30" customHeight="1" spans="3:14">
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -2202,11 +2145,10 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="O63" s="2"/>
-    </row>
-    <row r="64" ht="30" customHeight="1" spans="3:15">
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+    </row>
+    <row r="64" ht="30" customHeight="1" spans="3:14">
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2216,11 +2158,10 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="O64" s="2"/>
-    </row>
-    <row r="65" ht="30" customHeight="1" spans="3:15">
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+    </row>
+    <row r="65" ht="30" customHeight="1" spans="3:14">
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -2230,11 +2171,10 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="O65" s="2"/>
-    </row>
-    <row r="66" ht="30" customHeight="1" spans="3:15">
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+    </row>
+    <row r="66" ht="30" customHeight="1" spans="3:14">
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2244,11 +2184,10 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="O66" s="2"/>
-    </row>
-    <row r="67" ht="30" customHeight="1" spans="3:15">
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+    </row>
+    <row r="67" ht="30" customHeight="1" spans="3:14">
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -2258,11 +2197,10 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="O67" s="2"/>
-    </row>
-    <row r="68" ht="30" customHeight="1" spans="3:15">
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+    </row>
+    <row r="68" ht="30" customHeight="1" spans="3:14">
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2272,11 +2210,10 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="O68" s="2"/>
-    </row>
-    <row r="69" ht="30" customHeight="1" spans="3:15">
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+    </row>
+    <row r="69" ht="30" customHeight="1" spans="3:14">
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2286,11 +2223,10 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="O69" s="2"/>
-    </row>
-    <row r="70" ht="30" customHeight="1" spans="3:15">
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+    </row>
+    <row r="70" ht="30" customHeight="1" spans="3:14">
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -2300,11 +2236,10 @@
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="O70" s="2"/>
-    </row>
-    <row r="71" ht="30" customHeight="1" spans="3:15">
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+    </row>
+    <row r="71" ht="30" customHeight="1" spans="3:14">
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2314,11 +2249,10 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="O71" s="2"/>
-    </row>
-    <row r="72" ht="30" customHeight="1" spans="3:15">
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+    </row>
+    <row r="72" ht="30" customHeight="1" spans="3:14">
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -2328,11 +2262,10 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="O72" s="2"/>
-    </row>
-    <row r="73" ht="30" customHeight="1" spans="3:15">
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+    </row>
+    <row r="73" ht="30" customHeight="1" spans="3:14">
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -2342,11 +2275,10 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
-      <c r="M73" s="3"/>
-      <c r="O73" s="2"/>
-    </row>
-    <row r="74" ht="30" customHeight="1" spans="3:15">
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+    </row>
+    <row r="74" ht="30" customHeight="1" spans="3:14">
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -2356,11 +2288,10 @@
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-      <c r="O74" s="2"/>
-    </row>
-    <row r="75" ht="30" customHeight="1" spans="3:15">
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+    </row>
+    <row r="75" ht="30" customHeight="1" spans="3:14">
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -2370,11 +2301,10 @@
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="O75" s="2"/>
-    </row>
-    <row r="76" ht="30" customHeight="1" spans="3:15">
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+    </row>
+    <row r="76" ht="30" customHeight="1" spans="3:14">
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -2384,11 +2314,10 @@
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
-      <c r="O76" s="2"/>
-    </row>
-    <row r="77" ht="30" customHeight="1" spans="3:15">
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+    </row>
+    <row r="77" ht="30" customHeight="1" spans="3:14">
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -2398,11 +2327,10 @@
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="O77" s="2"/>
-    </row>
-    <row r="78" ht="30" customHeight="1" spans="3:15">
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+    </row>
+    <row r="78" ht="30" customHeight="1" spans="3:14">
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -2412,11 +2340,10 @@
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="O78" s="2"/>
-    </row>
-    <row r="79" ht="30" customHeight="1" spans="3:15">
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+    </row>
+    <row r="79" ht="30" customHeight="1" spans="3:14">
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -2426,11 +2353,10 @@
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="O79" s="2"/>
-    </row>
-    <row r="80" ht="30" customHeight="1" spans="3:15">
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+    </row>
+    <row r="80" ht="30" customHeight="1" spans="3:14">
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -2440,11 +2366,10 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="O80" s="2"/>
-    </row>
-    <row r="81" ht="30" customHeight="1" spans="3:15">
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+    </row>
+    <row r="81" ht="30" customHeight="1" spans="3:14">
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -2454,11 +2379,10 @@
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="O81" s="2"/>
-    </row>
-    <row r="82" ht="30" customHeight="1" spans="3:15">
+      <c r="M81" s="2"/>
+      <c r="N81" s="2"/>
+    </row>
+    <row r="82" ht="30" customHeight="1" spans="3:14">
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -2468,11 +2392,10 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
-      <c r="O82" s="2"/>
-    </row>
-    <row r="83" ht="30" customHeight="1" spans="3:15">
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+    </row>
+    <row r="83" ht="30" customHeight="1" spans="3:14">
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -2482,11 +2405,10 @@
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="O83" s="2"/>
-    </row>
-    <row r="84" ht="30" customHeight="1" spans="3:15">
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+    </row>
+    <row r="84" ht="30" customHeight="1" spans="3:14">
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -2496,11 +2418,10 @@
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="O84" s="2"/>
-    </row>
-    <row r="85" ht="30" customHeight="1" spans="3:15">
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+    </row>
+    <row r="85" ht="30" customHeight="1" spans="3:14">
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -2510,11 +2431,10 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
-      <c r="M85" s="3"/>
-      <c r="O85" s="2"/>
-    </row>
-    <row r="86" ht="30" customHeight="1" spans="3:15">
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+    </row>
+    <row r="86" ht="30" customHeight="1" spans="3:14">
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -2524,11 +2444,10 @@
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
-      <c r="O86" s="2"/>
-    </row>
-    <row r="87" ht="30" customHeight="1" spans="3:15">
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+    </row>
+    <row r="87" ht="30" customHeight="1" spans="3:14">
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -2538,11 +2457,10 @@
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3"/>
-      <c r="O87" s="2"/>
-    </row>
-    <row r="88" ht="30" customHeight="1" spans="3:15">
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+    </row>
+    <row r="88" ht="30" customHeight="1" spans="3:14">
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -2552,11 +2470,10 @@
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="O88" s="2"/>
-    </row>
-    <row r="89" ht="30" customHeight="1" spans="3:15">
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+    </row>
+    <row r="89" ht="30" customHeight="1" spans="3:14">
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -2566,11 +2483,10 @@
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
-      <c r="L89" s="3"/>
-      <c r="M89" s="3"/>
-      <c r="O89" s="2"/>
-    </row>
-    <row r="90" ht="30" customHeight="1" spans="3:15">
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+    </row>
+    <row r="90" ht="30" customHeight="1" spans="3:14">
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -2580,11 +2496,10 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="O90" s="2"/>
-    </row>
-    <row r="91" ht="30" customHeight="1" spans="3:15">
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+    </row>
+    <row r="91" ht="30" customHeight="1" spans="3:14">
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -2594,11 +2509,10 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
-      <c r="M91" s="3"/>
-      <c r="O91" s="2"/>
-    </row>
-    <row r="92" ht="30" customHeight="1" spans="3:15">
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+    </row>
+    <row r="92" ht="30" customHeight="1" spans="3:14">
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -2608,11 +2522,10 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="O92" s="2"/>
-    </row>
-    <row r="93" ht="30" customHeight="1" spans="3:15">
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+    </row>
+    <row r="93" ht="30" customHeight="1" spans="3:14">
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -2622,11 +2535,10 @@
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
-      <c r="L93" s="3"/>
-      <c r="M93" s="3"/>
-      <c r="O93" s="2"/>
-    </row>
-    <row r="94" ht="30" customHeight="1" spans="3:15">
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+    </row>
+    <row r="94" ht="30" customHeight="1" spans="3:14">
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -2636,11 +2548,10 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
-      <c r="L94" s="3"/>
-      <c r="M94" s="3"/>
-      <c r="O94" s="2"/>
-    </row>
-    <row r="95" ht="30" customHeight="1" spans="3:15">
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+    </row>
+    <row r="95" ht="30" customHeight="1" spans="3:14">
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -2650,11 +2561,10 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
-      <c r="M95" s="3"/>
-      <c r="O95" s="2"/>
-    </row>
-    <row r="96" ht="30" customHeight="1" spans="3:15">
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+    </row>
+    <row r="96" ht="30" customHeight="1" spans="3:14">
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -2664,11 +2574,10 @@
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="O96" s="2"/>
-    </row>
-    <row r="97" ht="30" customHeight="1" spans="3:15">
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+    </row>
+    <row r="97" ht="30" customHeight="1" spans="3:14">
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -2678,11 +2587,10 @@
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
-      <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="O97" s="2"/>
-    </row>
-    <row r="98" ht="30" customHeight="1" spans="3:15">
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+    </row>
+    <row r="98" ht="30" customHeight="1" spans="3:14">
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -2692,11 +2600,10 @@
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="O98" s="2"/>
-    </row>
-    <row r="99" ht="30" customHeight="1" spans="3:15">
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+    </row>
+    <row r="99" ht="30" customHeight="1" spans="3:14">
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -2706,11 +2613,10 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="O99" s="2"/>
-    </row>
-    <row r="100" ht="30" customHeight="1" spans="3:15">
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+    </row>
+    <row r="100" ht="30" customHeight="1" spans="3:14">
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -2720,11 +2626,10 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
-      <c r="L100" s="3"/>
-      <c r="M100" s="3"/>
-      <c r="O100" s="2"/>
-    </row>
-    <row r="101" ht="30" customHeight="1" spans="3:15">
+      <c r="M100" s="2"/>
+      <c r="N100" s="2"/>
+    </row>
+    <row r="101" ht="30" customHeight="1" spans="3:14">
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -2734,19 +2639,12 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="O101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Enter a valid number for Eligibility Age Max" sqref="K2:K101">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Enter a valid number for Mandatory Experience" sqref="L2:L101">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Enter a valid number for Preferred Experience" sqref="M2:M101">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Enter a valid number for Eligibility Age Min" sqref="I2:J101">

</xml_diff>